<commit_message>
T4.1 update bycatch case study
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Routput/Manuscript/bycatch case study/no. of citations bycatch PET case study.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Routput/Manuscript/bycatch case study/no. of citations bycatch PET case study.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="942">
   <si>
     <t xml:space="preserve">SW_ID</t>
   </si>
@@ -1971,30 +1971,6 @@
   </si>
   <si>
     <t xml:space="preserve">By-catch is one of the main sources of anthropogenic mortality in marine species of conservation concern worldwide. Between 2006 and 2008, the Consorzio Nazionale Interuniversitario per le Scienze del Mare (CoNISMa) coordinated a monitoring programme of cetacean by-catch in Italian pelagic trawlers, funded in compliance with European Regulation 812/2004. Sixteen independent observers monitored a total of 3141 hauls. The observation coverage ranged between 0.9 and 6.3% of the regional fishing effort. Almost all by-catch events were recorded in the northern Adriatic Sea. By-catch rates of bottlenose dolphins (Tursiops truncatus) and loggerhead turtles (Caretta caretta) were 0.0006 and 0.0255 individuals per haul, respectively. Given the low number of observed deaths, reliable estimates of total mortality for these two species were not obtained. The annual number of by-caught turtles was 863 (CV = 0.15), with 99% released alive. A 'hotspot' for turtle captures was found off Goro (south Venice). The existence of lethal interactions makes it important to understand whether the scale of this mortality is sufficient to pose a threat at population level. Finally, annual by-catch estimates for rays and sharks were 5436 (CV = 0.08) and 5414 (CV = 0.15), respectively. Thintail threshers (Alopias vulpinus), piked dogfish (Squalus acanthias) and smooth-hounds (Mustelus mustelus), which are both commercial and vulnerable to overfishing, were taken in large numbers. © 2010 Taylor &amp; Francis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW4_1184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crec'Hriou R., Alemany F., Roussel E., Chassanite A., Marinaro J.Y., Mader J., Rochel E., Planes S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fisheries replenishment of early life taxa: Potential export of fish eggs and larvae from a temperate marine protected area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fisheries Oceanography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1111/j.1365-2419.2010.00533.x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An ichthyoplankton survey was conducted at the periphery of Cabrera National Park (Balearic Islands, Western Mediterranean Sea) in July 2004, using bongo nets, fixed nets and collection of oceanographic data. This work focused on analysing the distribution of eggs and larval stages of some fishery-targeted taxa (Coris julis, Epinephelus spp., Sciaena umbra and Scorpaena sp.) whose adult abundances and/or biomass are higher in the reserve and therefore would be likely to show gradients of larval abundance attributable to the existence of the Marine Protected Area (MPA). Oceanographic data indicated there was water column stratification, horizontal distribution of surface water masses and hydrodynamic features linked with Mediterranean seasonality. During the summer sampling, eggs and larvae of targeted fish taxa were mainly located in the northeast of the MPA, near the coast. An effect of depth and current was demonstrated for Coris julis and Epinephelus spp. and there appears to be an offshore gradient for the other targeted taxa, especially for the egg stages. These data highlight the fact that the Cabrera archipelago is a potential important spawning area for targeted fishery species. © 2010 Blackwell Publishing Ltd.</t>
   </si>
   <si>
     <t xml:space="preserve">SW4_1185</t>
@@ -7599,10 +7575,10 @@
         <v>2010</v>
       </c>
       <c r="F84" t="s">
+        <v>441</v>
+      </c>
+      <c r="G84" t="s">
         <v>656</v>
-      </c>
-      <c r="G84" t="s">
-        <v>477</v>
       </c>
       <c r="H84" t="s">
         <v>90</v>
@@ -7632,7 +7608,7 @@
         <v>31</v>
       </c>
       <c r="Q84" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85">
@@ -7649,29 +7625,29 @@
         <v>663</v>
       </c>
       <c r="E85" t="n">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="F85" t="s">
-        <v>441</v>
+        <v>280</v>
       </c>
       <c r="G85" t="s">
-        <v>664</v>
+        <v>210</v>
       </c>
       <c r="H85" t="s">
         <v>90</v>
       </c>
       <c r="I85" t="s">
+        <v>664</v>
+      </c>
+      <c r="J85" t="s">
         <v>665</v>
       </c>
-      <c r="J85" t="s">
+      <c r="K85" t="s">
         <v>666</v>
       </c>
-      <c r="K85" t="s">
+      <c r="L85" t="s">
         <v>667</v>
       </c>
-      <c r="L85" t="s">
-        <v>668</v>
-      </c>
       <c r="M85" t="s">
         <v>28</v>
       </c>
@@ -7685,33 +7661,33 @@
         <v>31</v>
       </c>
       <c r="Q85" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>668</v>
+      </c>
+      <c r="B86" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" t="s">
         <v>669</v>
       </c>
-      <c r="B86" t="s">
-        <v>18</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>670</v>
-      </c>
-      <c r="D86" t="s">
-        <v>671</v>
       </c>
       <c r="E86" t="n">
         <v>2009</v>
       </c>
       <c r="F86" t="s">
-        <v>280</v>
+        <v>135</v>
       </c>
       <c r="G86" t="s">
+        <v>671</v>
+      </c>
+      <c r="H86" t="s">
         <v>210</v>
-      </c>
-      <c r="H86" t="s">
-        <v>90</v>
       </c>
       <c r="I86" t="s">
         <v>672</v>
@@ -7729,7 +7705,7 @@
         <v>28</v>
       </c>
       <c r="N86" t="s">
-        <v>29</v>
+        <v>603</v>
       </c>
       <c r="O86" t="s">
         <v>30</v>
@@ -7738,7 +7714,7 @@
         <v>31</v>
       </c>
       <c r="Q86" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87">
@@ -7758,72 +7734,72 @@
         <v>2009</v>
       </c>
       <c r="F87" t="s">
-        <v>135</v>
+        <v>325</v>
       </c>
       <c r="G87" t="s">
         <v>679</v>
       </c>
       <c r="H87" t="s">
-        <v>210</v>
+        <v>30</v>
       </c>
       <c r="I87" t="s">
         <v>680</v>
       </c>
       <c r="J87" t="s">
+        <v>233</v>
+      </c>
+      <c r="K87" t="s">
         <v>681</v>
       </c>
-      <c r="K87" t="s">
+      <c r="L87" t="s">
         <v>682</v>
       </c>
-      <c r="L87" t="s">
-        <v>683</v>
-      </c>
       <c r="M87" t="s">
         <v>28</v>
       </c>
       <c r="N87" t="s">
-        <v>603</v>
+        <v>29</v>
       </c>
       <c r="O87" t="s">
-        <v>30</v>
+        <v>261</v>
       </c>
       <c r="P87" t="s">
         <v>31</v>
       </c>
       <c r="Q87" t="n">
-        <v>33</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>683</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
         <v>684</v>
       </c>
-      <c r="B88" t="s">
-        <v>18</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>685</v>
-      </c>
-      <c r="D88" t="s">
-        <v>686</v>
       </c>
       <c r="E88" t="n">
         <v>2009</v>
       </c>
       <c r="F88" t="s">
-        <v>325</v>
+        <v>580</v>
       </c>
       <c r="G88" t="s">
+        <v>686</v>
+      </c>
+      <c r="H88" t="s">
+        <v>226</v>
+      </c>
+      <c r="I88" t="s">
         <v>687</v>
       </c>
-      <c r="H88" t="s">
-        <v>30</v>
-      </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>688</v>
-      </c>
-      <c r="J88" t="s">
-        <v>233</v>
       </c>
       <c r="K88" t="s">
         <v>689</v>
@@ -7835,113 +7811,113 @@
         <v>28</v>
       </c>
       <c r="N88" t="s">
-        <v>29</v>
+        <v>691</v>
       </c>
       <c r="O88" t="s">
-        <v>261</v>
+        <v>30</v>
       </c>
       <c r="P88" t="s">
         <v>31</v>
       </c>
       <c r="Q88" t="n">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B89" t="s">
         <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D89" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E89" t="n">
         <v>2009</v>
       </c>
       <c r="F89" t="s">
-        <v>580</v>
+        <v>695</v>
       </c>
       <c r="G89" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="H89" t="s">
-        <v>226</v>
+        <v>697</v>
       </c>
       <c r="I89" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="J89" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="K89" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="L89" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="M89" t="s">
         <v>28</v>
       </c>
       <c r="N89" t="s">
-        <v>699</v>
+        <v>29</v>
       </c>
       <c r="O89" t="s">
-        <v>30</v>
+        <v>261</v>
       </c>
       <c r="P89" t="s">
         <v>31</v>
       </c>
       <c r="Q89" t="n">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B90" t="s">
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="D90" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="E90" t="n">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="F90" t="s">
-        <v>703</v>
+        <v>505</v>
       </c>
       <c r="G90" t="s">
-        <v>704</v>
+        <v>105</v>
       </c>
       <c r="H90" t="s">
+        <v>66</v>
+      </c>
+      <c r="I90" t="s">
         <v>705</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
         <v>706</v>
       </c>
-      <c r="J90" t="s">
+      <c r="K90" t="s">
         <v>707</v>
       </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>708</v>
       </c>
-      <c r="L90" t="s">
-        <v>709</v>
-      </c>
       <c r="M90" t="s">
         <v>28</v>
       </c>
       <c r="N90" t="s">
-        <v>29</v>
+        <v>603</v>
       </c>
       <c r="O90" t="s">
         <v>261</v>
@@ -7950,33 +7926,33 @@
         <v>31</v>
       </c>
       <c r="Q90" t="n">
-        <v>94</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>709</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" t="s">
         <v>710</v>
       </c>
-      <c r="B91" t="s">
-        <v>18</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>711</v>
-      </c>
-      <c r="D91" t="s">
-        <v>712</v>
       </c>
       <c r="E91" t="n">
         <v>2008</v>
       </c>
       <c r="F91" t="s">
-        <v>505</v>
+        <v>111</v>
       </c>
       <c r="G91" t="s">
-        <v>105</v>
+        <v>380</v>
       </c>
       <c r="H91" t="s">
-        <v>66</v>
+        <v>712</v>
       </c>
       <c r="I91" t="s">
         <v>713</v>
@@ -7994,16 +7970,16 @@
         <v>28</v>
       </c>
       <c r="N91" t="s">
-        <v>603</v>
+        <v>29</v>
       </c>
       <c r="O91" t="s">
-        <v>261</v>
+        <v>30</v>
       </c>
       <c r="P91" t="s">
         <v>31</v>
       </c>
       <c r="Q91" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92">
@@ -8023,26 +7999,26 @@
         <v>2008</v>
       </c>
       <c r="F92" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="G92" t="s">
-        <v>380</v>
+        <v>622</v>
       </c>
       <c r="H92" t="s">
+        <v>127</v>
+      </c>
+      <c r="I92" t="s">
+        <v>373</v>
+      </c>
+      <c r="J92" t="s">
+        <v>374</v>
+      </c>
+      <c r="K92" t="s">
         <v>720</v>
       </c>
-      <c r="I92" t="s">
+      <c r="L92" t="s">
         <v>721</v>
       </c>
-      <c r="J92" t="s">
-        <v>722</v>
-      </c>
-      <c r="K92" t="s">
-        <v>723</v>
-      </c>
-      <c r="L92" t="s">
-        <v>724</v>
-      </c>
       <c r="M92" t="s">
         <v>28</v>
       </c>
@@ -8050,27 +8026,27 @@
         <v>29</v>
       </c>
       <c r="O92" t="s">
-        <v>30</v>
+        <v>427</v>
       </c>
       <c r="P92" t="s">
         <v>31</v>
       </c>
       <c r="Q92" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B93" t="s">
         <v>18</v>
       </c>
       <c r="C93" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D93" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E93" t="n">
         <v>2008</v>
@@ -8082,20 +8058,20 @@
         <v>622</v>
       </c>
       <c r="H93" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="I93" t="s">
-        <v>373</v>
+        <v>725</v>
       </c>
       <c r="J93" t="s">
-        <v>374</v>
+        <v>726</v>
       </c>
       <c r="K93" t="s">
+        <v>727</v>
+      </c>
+      <c r="L93" t="s">
         <v>728</v>
       </c>
-      <c r="L93" t="s">
-        <v>729</v>
-      </c>
       <c r="M93" t="s">
         <v>28</v>
       </c>
@@ -8103,52 +8079,52 @@
         <v>29</v>
       </c>
       <c r="O93" t="s">
-        <v>427</v>
+        <v>141</v>
       </c>
       <c r="P93" t="s">
         <v>31</v>
       </c>
       <c r="Q93" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>729</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
         <v>730</v>
       </c>
-      <c r="B94" t="s">
-        <v>18</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>731</v>
-      </c>
-      <c r="D94" t="s">
-        <v>732</v>
       </c>
       <c r="E94" t="n">
         <v>2008</v>
       </c>
       <c r="F94" t="s">
-        <v>135</v>
+        <v>363</v>
       </c>
       <c r="G94" t="s">
-        <v>622</v>
+        <v>732</v>
       </c>
       <c r="H94" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="I94" t="s">
+        <v>203</v>
+      </c>
+      <c r="J94" t="s">
+        <v>232</v>
+      </c>
+      <c r="K94" t="s">
         <v>733</v>
       </c>
-      <c r="J94" t="s">
+      <c r="L94" t="s">
         <v>734</v>
       </c>
-      <c r="K94" t="s">
-        <v>735</v>
-      </c>
-      <c r="L94" t="s">
-        <v>736</v>
-      </c>
       <c r="M94" t="s">
         <v>28</v>
       </c>
@@ -8156,51 +8132,51 @@
         <v>29</v>
       </c>
       <c r="O94" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P94" t="s">
         <v>31</v>
       </c>
       <c r="Q94" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>735</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" t="s">
+        <v>736</v>
+      </c>
+      <c r="D95" t="s">
         <v>737</v>
-      </c>
-      <c r="B95" t="s">
-        <v>18</v>
-      </c>
-      <c r="C95" t="s">
-        <v>738</v>
-      </c>
-      <c r="D95" t="s">
-        <v>739</v>
       </c>
       <c r="E95" t="n">
         <v>2008</v>
       </c>
       <c r="F95" t="s">
-        <v>363</v>
+        <v>738</v>
       </c>
       <c r="G95" t="s">
-        <v>740</v>
+        <v>82</v>
       </c>
       <c r="H95" t="s">
         <v>211</v>
       </c>
       <c r="I95" t="s">
-        <v>203</v>
+        <v>415</v>
       </c>
       <c r="J95" t="s">
-        <v>232</v>
+        <v>388</v>
       </c>
       <c r="K95" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="L95" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M95" t="s">
         <v>28</v>
@@ -8215,46 +8191,46 @@
         <v>31</v>
       </c>
       <c r="Q95" t="n">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>741</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>742</v>
+      </c>
+      <c r="D96" t="s">
         <v>743</v>
       </c>
-      <c r="B96" t="s">
-        <v>18</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="E96" t="n">
+        <v>2007</v>
+      </c>
+      <c r="F96" t="s">
+        <v>21</v>
+      </c>
+      <c r="G96" t="s">
+        <v>281</v>
+      </c>
+      <c r="H96" t="s">
+        <v>226</v>
+      </c>
+      <c r="I96" t="s">
         <v>744</v>
       </c>
-      <c r="D96" t="s">
+      <c r="J96" t="s">
         <v>745</v>
       </c>
-      <c r="E96" t="n">
-        <v>2008</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="K96" t="s">
         <v>746</v>
       </c>
-      <c r="G96" t="s">
-        <v>82</v>
-      </c>
-      <c r="H96" t="s">
-        <v>211</v>
-      </c>
-      <c r="I96" t="s">
-        <v>415</v>
-      </c>
-      <c r="J96" t="s">
-        <v>388</v>
-      </c>
-      <c r="K96" t="s">
+      <c r="L96" t="s">
         <v>747</v>
       </c>
-      <c r="L96" t="s">
-        <v>748</v>
-      </c>
       <c r="M96" t="s">
         <v>28</v>
       </c>
@@ -8268,33 +8244,33 @@
         <v>31</v>
       </c>
       <c r="Q96" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>748</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" t="s">
         <v>749</v>
       </c>
-      <c r="B97" t="s">
-        <v>18</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>750</v>
-      </c>
-      <c r="D97" t="s">
-        <v>751</v>
       </c>
       <c r="E97" t="n">
         <v>2007</v>
       </c>
       <c r="F97" t="s">
-        <v>21</v>
+        <v>441</v>
       </c>
       <c r="G97" t="s">
-        <v>281</v>
+        <v>751</v>
       </c>
       <c r="H97" t="s">
-        <v>226</v>
+        <v>97</v>
       </c>
       <c r="I97" t="s">
         <v>752</v>
@@ -8321,7 +8297,7 @@
         <v>31</v>
       </c>
       <c r="Q97" t="n">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98">
@@ -8341,19 +8317,19 @@
         <v>2007</v>
       </c>
       <c r="F98" t="s">
-        <v>441</v>
+        <v>42</v>
       </c>
       <c r="G98" t="s">
         <v>759</v>
       </c>
       <c r="H98" t="s">
-        <v>97</v>
+        <v>760</v>
       </c>
       <c r="I98" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="J98" t="s">
-        <v>761</v>
+        <v>725</v>
       </c>
       <c r="K98" t="s">
         <v>762</v>
@@ -8374,7 +8350,7 @@
         <v>31</v>
       </c>
       <c r="Q98" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99">
@@ -8394,26 +8370,26 @@
         <v>2007</v>
       </c>
       <c r="F99" t="s">
-        <v>42</v>
+        <v>767</v>
       </c>
       <c r="G99" t="s">
-        <v>767</v>
+        <v>281</v>
       </c>
       <c r="H99" t="s">
+        <v>90</v>
+      </c>
+      <c r="I99" t="s">
         <v>768</v>
       </c>
-      <c r="I99" t="s">
+      <c r="J99" t="s">
+        <v>395</v>
+      </c>
+      <c r="K99" t="s">
+        <v>30</v>
+      </c>
+      <c r="L99" t="s">
         <v>769</v>
       </c>
-      <c r="J99" t="s">
-        <v>733</v>
-      </c>
-      <c r="K99" t="s">
-        <v>770</v>
-      </c>
-      <c r="L99" t="s">
-        <v>771</v>
-      </c>
       <c r="M99" t="s">
         <v>28</v>
       </c>
@@ -8427,46 +8403,46 @@
         <v>31</v>
       </c>
       <c r="Q99" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>770</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" t="s">
+        <v>771</v>
+      </c>
+      <c r="D100" t="s">
         <v>772</v>
       </c>
-      <c r="B100" t="s">
-        <v>18</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="E100" t="n">
+        <v>2006</v>
+      </c>
+      <c r="F100" t="s">
+        <v>135</v>
+      </c>
+      <c r="G100" t="s">
+        <v>234</v>
+      </c>
+      <c r="H100" t="s">
+        <v>97</v>
+      </c>
+      <c r="I100" t="s">
         <v>773</v>
       </c>
-      <c r="D100" t="s">
+      <c r="J100" t="s">
         <v>774</v>
       </c>
-      <c r="E100" t="n">
-        <v>2007</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="K100" t="s">
         <v>775</v>
       </c>
-      <c r="G100" t="s">
-        <v>281</v>
-      </c>
-      <c r="H100" t="s">
-        <v>90</v>
-      </c>
-      <c r="I100" t="s">
+      <c r="L100" t="s">
         <v>776</v>
       </c>
-      <c r="J100" t="s">
-        <v>395</v>
-      </c>
-      <c r="K100" t="s">
-        <v>30</v>
-      </c>
-      <c r="L100" t="s">
-        <v>777</v>
-      </c>
       <c r="M100" t="s">
         <v>28</v>
       </c>
@@ -8474,42 +8450,42 @@
         <v>29</v>
       </c>
       <c r="O100" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="P100" t="s">
         <v>31</v>
       </c>
       <c r="Q100" t="n">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
+        <v>777</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
         <v>778</v>
       </c>
-      <c r="B101" t="s">
-        <v>18</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>779</v>
-      </c>
-      <c r="D101" t="s">
-        <v>780</v>
       </c>
       <c r="E101" t="n">
         <v>2006</v>
       </c>
       <c r="F101" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="G101" t="s">
+        <v>780</v>
+      </c>
+      <c r="H101" t="s">
+        <v>781</v>
+      </c>
+      <c r="I101" t="s">
         <v>234</v>
-      </c>
-      <c r="H101" t="s">
-        <v>97</v>
-      </c>
-      <c r="I101" t="s">
-        <v>781</v>
       </c>
       <c r="J101" t="s">
         <v>782</v>
@@ -8527,13 +8503,13 @@
         <v>29</v>
       </c>
       <c r="O101" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P101" t="s">
         <v>31</v>
       </c>
       <c r="Q101" t="n">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102">
@@ -8550,29 +8526,29 @@
         <v>787</v>
       </c>
       <c r="E102" t="n">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="F102" t="s">
-        <v>111</v>
+        <v>767</v>
       </c>
       <c r="G102" t="s">
         <v>788</v>
       </c>
       <c r="H102" t="s">
+        <v>66</v>
+      </c>
+      <c r="I102" t="s">
         <v>789</v>
       </c>
-      <c r="I102" t="s">
-        <v>234</v>
-      </c>
       <c r="J102" t="s">
+        <v>162</v>
+      </c>
+      <c r="K102" t="s">
+        <v>30</v>
+      </c>
+      <c r="L102" t="s">
         <v>790</v>
       </c>
-      <c r="K102" t="s">
-        <v>791</v>
-      </c>
-      <c r="L102" t="s">
-        <v>792</v>
-      </c>
       <c r="M102" t="s">
         <v>28</v>
       </c>
@@ -8586,45 +8562,45 @@
         <v>31</v>
       </c>
       <c r="Q102" t="n">
-        <v>193</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>791</v>
+      </c>
+      <c r="B103" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
+        <v>792</v>
+      </c>
+      <c r="D103" t="s">
         <v>793</v>
-      </c>
-      <c r="B103" t="s">
-        <v>18</v>
-      </c>
-      <c r="C103" t="s">
-        <v>794</v>
-      </c>
-      <c r="D103" t="s">
-        <v>795</v>
       </c>
       <c r="E103" t="n">
         <v>2005</v>
       </c>
       <c r="F103" t="s">
-        <v>775</v>
+        <v>580</v>
       </c>
       <c r="G103" t="s">
-        <v>796</v>
+        <v>174</v>
       </c>
       <c r="H103" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
       <c r="I103" t="s">
-        <v>797</v>
+        <v>622</v>
       </c>
       <c r="J103" t="s">
-        <v>162</v>
+        <v>431</v>
       </c>
       <c r="K103" t="s">
-        <v>30</v>
+        <v>794</v>
       </c>
       <c r="L103" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="M103" t="s">
         <v>28</v>
@@ -8639,45 +8615,45 @@
         <v>31</v>
       </c>
       <c r="Q103" t="n">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="B104" t="s">
         <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D104" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="E104" t="n">
         <v>2005</v>
       </c>
       <c r="F104" t="s">
-        <v>580</v>
+        <v>799</v>
       </c>
       <c r="G104" t="s">
-        <v>174</v>
+        <v>800</v>
       </c>
       <c r="H104" t="s">
-        <v>211</v>
+        <v>30</v>
       </c>
       <c r="I104" t="s">
-        <v>622</v>
+        <v>801</v>
       </c>
       <c r="J104" t="s">
-        <v>431</v>
+        <v>802</v>
       </c>
       <c r="K104" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="L104" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="M104" t="s">
         <v>28</v>
@@ -8686,52 +8662,52 @@
         <v>29</v>
       </c>
       <c r="O104" t="s">
-        <v>30</v>
+        <v>427</v>
       </c>
       <c r="P104" t="s">
         <v>31</v>
       </c>
       <c r="Q104" t="n">
-        <v>71</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B105" t="s">
         <v>18</v>
       </c>
       <c r="C105" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D105" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E105" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="F105" t="s">
-        <v>807</v>
+        <v>580</v>
       </c>
       <c r="G105" t="s">
+        <v>484</v>
+      </c>
+      <c r="H105" t="s">
+        <v>66</v>
+      </c>
+      <c r="I105" t="s">
         <v>808</v>
       </c>
-      <c r="H105" t="s">
-        <v>30</v>
-      </c>
-      <c r="I105" t="s">
+      <c r="J105" t="s">
         <v>809</v>
       </c>
-      <c r="J105" t="s">
+      <c r="K105" t="s">
         <v>810</v>
       </c>
-      <c r="K105" t="s">
+      <c r="L105" t="s">
         <v>811</v>
       </c>
-      <c r="L105" t="s">
-        <v>812</v>
-      </c>
       <c r="M105" t="s">
         <v>28</v>
       </c>
@@ -8739,42 +8715,42 @@
         <v>29</v>
       </c>
       <c r="O105" t="s">
-        <v>427</v>
+        <v>30</v>
       </c>
       <c r="P105" t="s">
         <v>31</v>
       </c>
       <c r="Q105" t="n">
-        <v>14</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
+        <v>812</v>
+      </c>
+      <c r="B106" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" t="s">
         <v>813</v>
       </c>
-      <c r="B106" t="s">
-        <v>18</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>814</v>
-      </c>
-      <c r="D106" t="s">
-        <v>815</v>
       </c>
       <c r="E106" t="n">
         <v>2004</v>
       </c>
       <c r="F106" t="s">
-        <v>580</v>
+        <v>815</v>
       </c>
       <c r="G106" t="s">
-        <v>484</v>
+        <v>355</v>
       </c>
       <c r="H106" t="s">
-        <v>66</v>
+        <v>816</v>
       </c>
       <c r="I106" t="s">
-        <v>816</v>
+        <v>664</v>
       </c>
       <c r="J106" t="s">
         <v>817</v>
@@ -8798,7 +8774,7 @@
         <v>31</v>
       </c>
       <c r="Q106" t="n">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="107">
@@ -8818,16 +8794,16 @@
         <v>2004</v>
       </c>
       <c r="F107" t="s">
+        <v>580</v>
+      </c>
+      <c r="G107" t="s">
         <v>823</v>
       </c>
-      <c r="G107" t="s">
-        <v>355</v>
-      </c>
       <c r="H107" t="s">
+        <v>66</v>
+      </c>
+      <c r="I107" t="s">
         <v>824</v>
-      </c>
-      <c r="I107" t="s">
-        <v>672</v>
       </c>
       <c r="J107" t="s">
         <v>825</v>
@@ -8851,7 +8827,7 @@
         <v>31</v>
       </c>
       <c r="Q107" t="n">
-        <v>111</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108">
@@ -8868,29 +8844,29 @@
         <v>830</v>
       </c>
       <c r="E108" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="F108" t="s">
-        <v>580</v>
+        <v>799</v>
       </c>
       <c r="G108" t="s">
+        <v>22</v>
+      </c>
+      <c r="H108" t="s">
+        <v>30</v>
+      </c>
+      <c r="I108" t="s">
+        <v>726</v>
+      </c>
+      <c r="J108" t="s">
         <v>831</v>
       </c>
-      <c r="H108" t="s">
-        <v>66</v>
-      </c>
-      <c r="I108" t="s">
+      <c r="K108" t="s">
         <v>832</v>
       </c>
-      <c r="J108" t="s">
+      <c r="L108" t="s">
         <v>833</v>
       </c>
-      <c r="K108" t="s">
-        <v>834</v>
-      </c>
-      <c r="L108" t="s">
-        <v>835</v>
-      </c>
       <c r="M108" t="s">
         <v>28</v>
       </c>
@@ -8898,42 +8874,42 @@
         <v>29</v>
       </c>
       <c r="O108" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="P108" t="s">
         <v>31</v>
       </c>
       <c r="Q108" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
+        <v>834</v>
+      </c>
+      <c r="B109" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" t="s">
+        <v>835</v>
+      </c>
+      <c r="D109" t="s">
         <v>836</v>
       </c>
-      <c r="B109" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="E109" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F109" t="s">
+        <v>334</v>
+      </c>
+      <c r="G109" t="s">
         <v>837</v>
       </c>
-      <c r="D109" t="s">
+      <c r="H109" t="s">
+        <v>181</v>
+      </c>
+      <c r="I109" t="s">
         <v>838</v>
-      </c>
-      <c r="E109" t="n">
-        <v>2003</v>
-      </c>
-      <c r="F109" t="s">
-        <v>807</v>
-      </c>
-      <c r="G109" t="s">
-        <v>22</v>
-      </c>
-      <c r="H109" t="s">
-        <v>30</v>
-      </c>
-      <c r="I109" t="s">
-        <v>734</v>
       </c>
       <c r="J109" t="s">
         <v>839</v>
@@ -8951,13 +8927,13 @@
         <v>29</v>
       </c>
       <c r="O109" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P109" t="s">
         <v>31</v>
       </c>
       <c r="Q109" t="n">
-        <v>27</v>
+        <v>199</v>
       </c>
     </row>
     <row r="110">
@@ -8977,26 +8953,26 @@
         <v>2002</v>
       </c>
       <c r="F110" t="s">
-        <v>334</v>
+        <v>135</v>
       </c>
       <c r="G110" t="s">
+        <v>780</v>
+      </c>
+      <c r="H110" t="s">
+        <v>127</v>
+      </c>
+      <c r="I110" t="s">
         <v>845</v>
       </c>
-      <c r="H110" t="s">
-        <v>181</v>
-      </c>
-      <c r="I110" t="s">
+      <c r="J110" t="s">
+        <v>137</v>
+      </c>
+      <c r="K110" t="s">
         <v>846</v>
       </c>
-      <c r="J110" t="s">
+      <c r="L110" t="s">
         <v>847</v>
       </c>
-      <c r="K110" t="s">
-        <v>848</v>
-      </c>
-      <c r="L110" t="s">
-        <v>849</v>
-      </c>
       <c r="M110" t="s">
         <v>28</v>
       </c>
@@ -9004,52 +8980,52 @@
         <v>29</v>
       </c>
       <c r="O110" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="P110" t="s">
         <v>31</v>
       </c>
       <c r="Q110" t="n">
-        <v>199</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>848</v>
+      </c>
+      <c r="B111" t="s">
+        <v>18</v>
+      </c>
+      <c r="C111" t="s">
+        <v>849</v>
+      </c>
+      <c r="D111" t="s">
         <v>850</v>
       </c>
-      <c r="B111" t="s">
-        <v>18</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="E111" t="n">
+        <v>1998</v>
+      </c>
+      <c r="F111" t="s">
         <v>851</v>
       </c>
-      <c r="D111" t="s">
+      <c r="G111" t="s">
         <v>852</v>
       </c>
-      <c r="E111" t="n">
-        <v>2002</v>
-      </c>
-      <c r="F111" t="s">
-        <v>135</v>
-      </c>
-      <c r="G111" t="s">
-        <v>788</v>
-      </c>
       <c r="H111" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="I111" t="s">
+        <v>211</v>
+      </c>
+      <c r="J111" t="s">
+        <v>57</v>
+      </c>
+      <c r="K111" t="s">
+        <v>30</v>
+      </c>
+      <c r="L111" t="s">
         <v>853</v>
       </c>
-      <c r="J111" t="s">
-        <v>137</v>
-      </c>
-      <c r="K111" t="s">
-        <v>854</v>
-      </c>
-      <c r="L111" t="s">
-        <v>855</v>
-      </c>
       <c r="M111" t="s">
         <v>28</v>
       </c>
@@ -9057,48 +9033,48 @@
         <v>29</v>
       </c>
       <c r="O111" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P111" t="s">
         <v>31</v>
       </c>
       <c r="Q111" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>854</v>
+      </c>
+      <c r="B112" t="s">
+        <v>18</v>
+      </c>
+      <c r="C112" t="s">
+        <v>855</v>
+      </c>
+      <c r="D112" t="s">
         <v>856</v>
-      </c>
-      <c r="B112" t="s">
-        <v>18</v>
-      </c>
-      <c r="C112" t="s">
-        <v>857</v>
-      </c>
-      <c r="D112" t="s">
-        <v>858</v>
       </c>
       <c r="E112" t="n">
         <v>1998</v>
       </c>
       <c r="F112" t="s">
-        <v>859</v>
+        <v>363</v>
       </c>
       <c r="G112" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="H112" t="s">
         <v>211</v>
       </c>
       <c r="I112" t="s">
-        <v>211</v>
+        <v>858</v>
       </c>
       <c r="J112" t="s">
-        <v>57</v>
+        <v>859</v>
       </c>
       <c r="K112" t="s">
-        <v>30</v>
+        <v>860</v>
       </c>
       <c r="L112" t="s">
         <v>861</v>
@@ -9116,7 +9092,7 @@
         <v>31</v>
       </c>
       <c r="Q112" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="113">
@@ -9136,13 +9112,13 @@
         <v>1998</v>
       </c>
       <c r="F113" t="s">
-        <v>363</v>
+        <v>865</v>
       </c>
       <c r="G113" t="s">
-        <v>865</v>
+        <v>622</v>
       </c>
       <c r="H113" t="s">
-        <v>211</v>
+        <v>30</v>
       </c>
       <c r="I113" t="s">
         <v>866</v>
@@ -9169,7 +9145,7 @@
         <v>31</v>
       </c>
       <c r="Q113" t="n">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="114">
@@ -9189,26 +9165,26 @@
         <v>1998</v>
       </c>
       <c r="F114" t="s">
+        <v>135</v>
+      </c>
+      <c r="G114" t="s">
         <v>873</v>
       </c>
-      <c r="G114" t="s">
-        <v>622</v>
-      </c>
       <c r="H114" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="I114" t="s">
+        <v>635</v>
+      </c>
+      <c r="J114" t="s">
         <v>874</v>
       </c>
-      <c r="J114" t="s">
+      <c r="K114" t="s">
         <v>875</v>
       </c>
-      <c r="K114" t="s">
+      <c r="L114" t="s">
         <v>876</v>
       </c>
-      <c r="L114" t="s">
-        <v>877</v>
-      </c>
       <c r="M114" t="s">
         <v>28</v>
       </c>
@@ -9216,27 +9192,27 @@
         <v>29</v>
       </c>
       <c r="O114" t="s">
-        <v>30</v>
+        <v>427</v>
       </c>
       <c r="P114" t="s">
         <v>31</v>
       </c>
       <c r="Q114" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
+        <v>877</v>
+      </c>
+      <c r="B115" t="s">
+        <v>18</v>
+      </c>
+      <c r="C115" t="s">
         <v>878</v>
       </c>
-      <c r="B115" t="s">
-        <v>18</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>879</v>
-      </c>
-      <c r="D115" t="s">
-        <v>880</v>
       </c>
       <c r="E115" t="n">
         <v>1998</v>
@@ -9245,129 +9221,129 @@
         <v>135</v>
       </c>
       <c r="G115" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="H115" t="s">
         <v>66</v>
       </c>
       <c r="I115" t="s">
-        <v>635</v>
+        <v>880</v>
       </c>
       <c r="J115" t="s">
+        <v>356</v>
+      </c>
+      <c r="K115" t="s">
+        <v>881</v>
+      </c>
+      <c r="L115" t="s">
         <v>882</v>
       </c>
-      <c r="K115" t="s">
-        <v>883</v>
-      </c>
-      <c r="L115" t="s">
-        <v>884</v>
-      </c>
       <c r="M115" t="s">
         <v>28</v>
       </c>
       <c r="N115" t="s">
-        <v>29</v>
+        <v>603</v>
       </c>
       <c r="O115" t="s">
-        <v>427</v>
+        <v>141</v>
       </c>
       <c r="P115" t="s">
         <v>31</v>
       </c>
       <c r="Q115" t="n">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
+        <v>883</v>
+      </c>
+      <c r="B116" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116" t="s">
+        <v>884</v>
+      </c>
+      <c r="D116" t="s">
         <v>885</v>
       </c>
-      <c r="B116" t="s">
-        <v>18</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="E116" t="n">
+        <v>1997</v>
+      </c>
+      <c r="F116" t="s">
         <v>886</v>
       </c>
-      <c r="D116" t="s">
+      <c r="G116" t="s">
+        <v>680</v>
+      </c>
+      <c r="H116" t="s">
+        <v>127</v>
+      </c>
+      <c r="I116" t="s">
+        <v>726</v>
+      </c>
+      <c r="J116" t="s">
+        <v>831</v>
+      </c>
+      <c r="K116" t="s">
+        <v>30</v>
+      </c>
+      <c r="L116" t="s">
         <v>887</v>
       </c>
-      <c r="E116" t="n">
-        <v>1998</v>
-      </c>
-      <c r="F116" t="s">
-        <v>135</v>
-      </c>
-      <c r="G116" t="s">
-        <v>881</v>
-      </c>
-      <c r="H116" t="s">
-        <v>66</v>
-      </c>
-      <c r="I116" t="s">
-        <v>888</v>
-      </c>
-      <c r="J116" t="s">
-        <v>356</v>
-      </c>
-      <c r="K116" t="s">
-        <v>889</v>
-      </c>
-      <c r="L116" t="s">
-        <v>890</v>
-      </c>
       <c r="M116" t="s">
         <v>28</v>
       </c>
       <c r="N116" t="s">
-        <v>603</v>
+        <v>29</v>
       </c>
       <c r="O116" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P116" t="s">
         <v>31</v>
       </c>
       <c r="Q116" t="n">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="B117" t="s">
         <v>18</v>
       </c>
       <c r="C117" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="D117" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="E117" t="n">
         <v>1997</v>
       </c>
       <c r="F117" t="s">
+        <v>135</v>
+      </c>
+      <c r="G117" t="s">
+        <v>545</v>
+      </c>
+      <c r="H117" t="s">
+        <v>97</v>
+      </c>
+      <c r="I117" t="s">
+        <v>891</v>
+      </c>
+      <c r="J117" t="s">
+        <v>892</v>
+      </c>
+      <c r="K117" t="s">
+        <v>893</v>
+      </c>
+      <c r="L117" t="s">
         <v>894</v>
       </c>
-      <c r="G117" t="s">
-        <v>688</v>
-      </c>
-      <c r="H117" t="s">
-        <v>127</v>
-      </c>
-      <c r="I117" t="s">
-        <v>734</v>
-      </c>
-      <c r="J117" t="s">
-        <v>839</v>
-      </c>
-      <c r="K117" t="s">
-        <v>30</v>
-      </c>
-      <c r="L117" t="s">
-        <v>895</v>
-      </c>
       <c r="M117" t="s">
         <v>28</v>
       </c>
@@ -9375,52 +9351,52 @@
         <v>29</v>
       </c>
       <c r="O117" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="P117" t="s">
         <v>31</v>
       </c>
       <c r="Q117" t="n">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
+        <v>895</v>
+      </c>
+      <c r="B118" t="s">
+        <v>18</v>
+      </c>
+      <c r="C118" t="s">
         <v>896</v>
       </c>
-      <c r="B118" t="s">
-        <v>18</v>
-      </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>897</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="n">
+        <v>1996</v>
+      </c>
+      <c r="F118" t="s">
         <v>898</v>
       </c>
-      <c r="E118" t="n">
-        <v>1997</v>
-      </c>
-      <c r="F118" t="s">
-        <v>135</v>
-      </c>
       <c r="G118" t="s">
-        <v>545</v>
+        <v>899</v>
       </c>
       <c r="H118" t="s">
-        <v>97</v>
+        <v>781</v>
       </c>
       <c r="I118" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J118" t="s">
-        <v>900</v>
+        <v>395</v>
       </c>
       <c r="K118" t="s">
+        <v>30</v>
+      </c>
+      <c r="L118" t="s">
         <v>901</v>
       </c>
-      <c r="L118" t="s">
-        <v>902</v>
-      </c>
       <c r="M118" t="s">
         <v>28</v>
       </c>
@@ -9428,48 +9404,48 @@
         <v>29</v>
       </c>
       <c r="O118" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P118" t="s">
         <v>31</v>
       </c>
       <c r="Q118" t="n">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>902</v>
+      </c>
+      <c r="B119" t="s">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
         <v>903</v>
       </c>
-      <c r="B119" t="s">
-        <v>18</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>904</v>
-      </c>
-      <c r="D119" t="s">
-        <v>905</v>
       </c>
       <c r="E119" t="n">
         <v>1996</v>
       </c>
       <c r="F119" t="s">
+        <v>135</v>
+      </c>
+      <c r="G119" t="s">
+        <v>905</v>
+      </c>
+      <c r="H119" t="s">
+        <v>181</v>
+      </c>
+      <c r="I119" t="s">
         <v>906</v>
       </c>
-      <c r="G119" t="s">
+      <c r="J119" t="s">
         <v>907</v>
       </c>
-      <c r="H119" t="s">
-        <v>789</v>
-      </c>
-      <c r="I119" t="s">
+      <c r="K119" t="s">
         <v>908</v>
-      </c>
-      <c r="J119" t="s">
-        <v>395</v>
-      </c>
-      <c r="K119" t="s">
-        <v>30</v>
       </c>
       <c r="L119" t="s">
         <v>909</v>
@@ -9481,13 +9457,13 @@
         <v>29</v>
       </c>
       <c r="O119" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="P119" t="s">
         <v>31</v>
       </c>
       <c r="Q119" t="n">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120">
@@ -9504,25 +9480,25 @@
         <v>912</v>
       </c>
       <c r="E120" t="n">
-        <v>1996</v>
+        <v>1992</v>
       </c>
       <c r="F120" t="s">
-        <v>135</v>
+        <v>913</v>
       </c>
       <c r="G120" t="s">
-        <v>913</v>
+        <v>468</v>
       </c>
       <c r="H120" t="s">
-        <v>181</v>
+        <v>914</v>
       </c>
       <c r="I120" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="J120" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="K120" t="s">
-        <v>916</v>
+        <v>30</v>
       </c>
       <c r="L120" t="s">
         <v>917</v>
@@ -9534,13 +9510,13 @@
         <v>29</v>
       </c>
       <c r="O120" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="P120" t="s">
         <v>31</v>
       </c>
       <c r="Q120" t="n">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121">
@@ -9557,81 +9533,81 @@
         <v>920</v>
       </c>
       <c r="E121" t="n">
-        <v>1992</v>
+        <v>2018</v>
       </c>
       <c r="F121" t="s">
         <v>921</v>
       </c>
       <c r="G121" t="s">
-        <v>468</v>
+        <v>800</v>
       </c>
       <c r="H121" t="s">
+        <v>66</v>
+      </c>
+      <c r="I121" t="s">
+        <v>490</v>
+      </c>
+      <c r="J121" t="s">
         <v>922</v>
       </c>
-      <c r="I121" t="s">
+      <c r="K121" t="s">
         <v>923</v>
       </c>
-      <c r="J121" t="s">
+      <c r="L121" t="s">
         <v>924</v>
       </c>
-      <c r="K121" t="s">
-        <v>30</v>
-      </c>
-      <c r="L121" t="s">
+      <c r="M121" t="s">
+        <v>28</v>
+      </c>
+      <c r="N121" t="s">
+        <v>29</v>
+      </c>
+      <c r="O121" t="s">
         <v>925</v>
       </c>
-      <c r="M121" t="s">
-        <v>28</v>
-      </c>
-      <c r="N121" t="s">
-        <v>29</v>
-      </c>
-      <c r="O121" t="s">
-        <v>30</v>
-      </c>
       <c r="P121" t="s">
-        <v>31</v>
+        <v>926</v>
       </c>
       <c r="Q121" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B122" t="s">
         <v>18</v>
       </c>
       <c r="C122" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D122" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="E122" t="n">
         <v>2018</v>
       </c>
       <c r="F122" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="G122" t="s">
-        <v>808</v>
+        <v>780</v>
       </c>
       <c r="H122" t="s">
-        <v>66</v>
+        <v>181</v>
       </c>
       <c r="I122" t="s">
-        <v>490</v>
+        <v>931</v>
       </c>
       <c r="J122" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="K122" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="L122" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="M122" t="s">
         <v>28</v>
@@ -9639,14 +9615,12 @@
       <c r="N122" t="s">
         <v>29</v>
       </c>
-      <c r="O122" t="s">
-        <v>933</v>
-      </c>
+      <c r="O122"/>
       <c r="P122" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="Q122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -9666,25 +9640,25 @@
         <v>2018</v>
       </c>
       <c r="F123" t="s">
+        <v>930</v>
+      </c>
+      <c r="G123" t="s">
+        <v>780</v>
+      </c>
+      <c r="H123" t="s">
+        <v>97</v>
+      </c>
+      <c r="I123" t="s">
         <v>938</v>
       </c>
-      <c r="G123" t="s">
-        <v>788</v>
-      </c>
-      <c r="H123" t="s">
-        <v>181</v>
-      </c>
-      <c r="I123" t="s">
+      <c r="J123" t="s">
         <v>939</v>
       </c>
-      <c r="J123" t="s">
+      <c r="K123" t="s">
         <v>940</v>
       </c>
-      <c r="K123" t="s">
+      <c r="L123" t="s">
         <v>941</v>
-      </c>
-      <c r="L123" t="s">
-        <v>942</v>
       </c>
       <c r="M123" t="s">
         <v>28</v>
@@ -9694,60 +9668,9 @@
       </c>
       <c r="O123"/>
       <c r="P123" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="Q123" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s">
-        <v>943</v>
-      </c>
-      <c r="B124" t="s">
-        <v>18</v>
-      </c>
-      <c r="C124" t="s">
-        <v>944</v>
-      </c>
-      <c r="D124" t="s">
-        <v>945</v>
-      </c>
-      <c r="E124" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F124" t="s">
-        <v>938</v>
-      </c>
-      <c r="G124" t="s">
-        <v>788</v>
-      </c>
-      <c r="H124" t="s">
-        <v>97</v>
-      </c>
-      <c r="I124" t="s">
-        <v>946</v>
-      </c>
-      <c r="J124" t="s">
-        <v>947</v>
-      </c>
-      <c r="K124" t="s">
-        <v>948</v>
-      </c>
-      <c r="L124" t="s">
-        <v>949</v>
-      </c>
-      <c r="M124" t="s">
-        <v>28</v>
-      </c>
-      <c r="N124" t="s">
-        <v>29</v>
-      </c>
-      <c r="O124"/>
-      <c r="P124" t="s">
-        <v>934</v>
-      </c>
-      <c r="Q124" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>